<commit_message>
Uploaded the new version of the Build list
</commit_message>
<xml_diff>
--- a/BuildList.xlsx
+++ b/BuildList.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14655" windowHeight="5790"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="694" uniqueCount="532">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="697" uniqueCount="535">
   <si>
     <t>Region Name</t>
   </si>
@@ -1615,6 +1615,15 @@
   </si>
   <si>
     <t>Farm (2x Reed )</t>
+  </si>
+  <si>
+    <t>Army Slot 1</t>
+  </si>
+  <si>
+    <t>Army Slot 2</t>
+  </si>
+  <si>
+    <t>Trading Company Slot</t>
   </si>
 </sst>
 </file>
@@ -1689,7 +1698,22 @@
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="11">
+  <dxfs count="16">
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -1737,24 +1761,30 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabelle1" displayName="Tabelle1" ref="A1:I350" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
-  <autoFilter ref="A1:I350">
-    <filterColumn colId="2">
-      <customFilters>
-        <customFilter operator="notEqual" val=" "/>
-      </customFilters>
-    </filterColumn>
-  </autoFilter>
-  <tableColumns count="9">
-    <tableColumn id="1" name="Region Number" dataDxfId="8"/>
-    <tableColumn id="2" name="Region Name" dataDxfId="7"/>
-    <tableColumn id="3" name="Claimed by" dataDxfId="6"/>
-    <tableColumn id="4" name="Type of Claimbuild" dataDxfId="5"/>
-    <tableColumn id="5" name="Claimbuild Name" dataDxfId="4"/>
-    <tableColumn id="6" name="Coordinates" dataDxfId="3"/>
-    <tableColumn id="7" name="Trader" dataDxfId="2"/>
-    <tableColumn id="8" name="Ressources" dataDxfId="1"/>
-    <tableColumn id="9" name="Build by" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabelle1" displayName="Tabelle1" ref="A1:K350" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14">
+  <autoFilter ref="A1:K350"/>
+  <tableColumns count="11">
+    <tableColumn id="1" name="Region Number" dataDxfId="13"/>
+    <tableColumn id="2" name="Region Name" dataDxfId="12"/>
+    <tableColumn id="3" name="Claimed by" dataDxfId="11"/>
+    <tableColumn id="4" name="Type of Claimbuild" dataDxfId="10"/>
+    <tableColumn id="5" name="Claimbuild Name" dataDxfId="9"/>
+    <tableColumn id="6" name="Coordinates" dataDxfId="8"/>
+    <tableColumn id="7" name="Trader" dataDxfId="7"/>
+    <tableColumn id="8" name="Ressources" dataDxfId="6"/>
+    <tableColumn id="9" name="Army Slot 1" dataDxfId="5"/>
+    <tableColumn id="10" name="Army Slot 2" dataDxfId="4"/>
+    <tableColumn id="11" name="Trading Company Slot" dataDxfId="3"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium18" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabelle2" displayName="Tabelle2" ref="L1:L350" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1">
+  <autoFilter ref="L1:L350"/>
+  <tableColumns count="1">
+    <tableColumn id="1" name="Build by" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium18" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2023,10 +2053,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I350"/>
+  <dimension ref="A1:L350"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A153" sqref="A153:I154"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2039,10 +2069,13 @@
     <col min="6" max="6" width="17.85546875" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="28.28515625" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="43" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.140625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>82</v>
       </c>
@@ -2067,331 +2100,420 @@
       <c r="H1" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" t="s">
+        <v>532</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>533</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>534</v>
+      </c>
+      <c r="L1" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J10" s="2"/>
+      <c r="K10" s="2"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J11" s="2"/>
+      <c r="K11" s="2"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>11</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J12" s="2"/>
+      <c r="K12" s="2"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>12</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J13" s="2"/>
+      <c r="K13" s="2"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>13</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J14" s="2"/>
+      <c r="K14" s="2"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>14</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J15" s="2"/>
+      <c r="K15" s="2"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>15</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J16" s="2"/>
+      <c r="K16" s="2"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>16</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J17" s="2"/>
+      <c r="K17" s="2"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>17</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J18" s="2"/>
+      <c r="K18" s="2"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>18</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J19" s="2"/>
+      <c r="K19" s="2"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>19</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J20" s="2"/>
+      <c r="K20" s="2"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>20</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J21" s="2"/>
+      <c r="K21" s="2"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>21</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J22" s="2"/>
+      <c r="K22" s="2"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>22</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J23" s="2"/>
+      <c r="K23" s="2"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>23</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J24" s="2"/>
+      <c r="K24" s="2"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>24</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J25" s="2"/>
+      <c r="K25" s="2"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>25</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J26" s="2"/>
+      <c r="K26" s="2"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>26</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J27" s="2"/>
+      <c r="K27" s="2"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>27</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J28" s="2"/>
+      <c r="K28" s="2"/>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <v>28</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J29" s="2"/>
+      <c r="K29" s="2"/>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <v>29</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J30" s="2"/>
+      <c r="K30" s="2"/>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <v>30</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J31" s="2"/>
+      <c r="K31" s="2"/>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <v>31</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="33" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J32" s="2"/>
+      <c r="K32" s="2"/>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
         <v>32</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="34" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J33" s="2"/>
+      <c r="K33" s="2"/>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
         <v>33</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="35" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J34" s="2"/>
+      <c r="K34" s="2"/>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
         <v>34</v>
       </c>
       <c r="B35" s="2" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="36" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J35" s="2"/>
+      <c r="K35" s="2"/>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
         <v>35</v>
       </c>
       <c r="B36" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="37" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J36" s="2"/>
+      <c r="K36" s="2"/>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
         <v>36</v>
       </c>
       <c r="B37" s="2" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="38" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J37" s="2"/>
+      <c r="K37" s="2"/>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
         <v>37</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="39" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J38" s="2"/>
+      <c r="K38" s="2"/>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
         <v>38</v>
       </c>
       <c r="B39" s="2" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="40" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J39" s="2"/>
+      <c r="K39" s="2"/>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
         <v>39</v>
       </c>
       <c r="B40" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="41" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J40" s="2"/>
+      <c r="K40" s="2"/>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
         <v>40</v>
       </c>
       <c r="B41" s="2" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J41" s="2"/>
+      <c r="K41" s="2"/>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
         <v>41</v>
       </c>
@@ -2413,27 +2535,33 @@
       <c r="G42" s="2" t="s">
         <v>464</v>
       </c>
-      <c r="I42" s="2" t="s">
+      <c r="J42" s="2"/>
+      <c r="K42" s="2"/>
+      <c r="L42" s="2" t="s">
         <v>351</v>
       </c>
     </row>
-    <row r="43" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
         <v>42</v>
       </c>
       <c r="B43" s="2" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="44" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J43" s="2"/>
+      <c r="K43" s="2"/>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" s="2">
         <v>43</v>
       </c>
       <c r="B44" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J44" s="2"/>
+      <c r="K44" s="2"/>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" s="2">
         <v>44</v>
       </c>
@@ -2452,131 +2580,163 @@
       <c r="F45" s="2" t="s">
         <v>347</v>
       </c>
-      <c r="I45" s="2" t="s">
+      <c r="J45" s="2"/>
+      <c r="K45" s="2"/>
+      <c r="L45" s="2" t="s">
         <v>348</v>
       </c>
     </row>
-    <row r="46" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46" s="2">
         <v>45</v>
       </c>
       <c r="B46" s="2" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="47" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J46" s="2"/>
+      <c r="K46" s="2"/>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47" s="2">
         <v>46</v>
       </c>
       <c r="B47" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="48" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J47" s="2"/>
+      <c r="K47" s="2"/>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48" s="2">
         <v>47</v>
       </c>
       <c r="B48" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="49" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J48" s="2"/>
+      <c r="K48" s="2"/>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A49" s="2">
         <v>48</v>
       </c>
       <c r="B49" s="2" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="50" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J49" s="2"/>
+      <c r="K49" s="2"/>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A50" s="2">
         <v>49</v>
       </c>
       <c r="B50" s="2" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="51" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J50" s="2"/>
+      <c r="K50" s="2"/>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A51" s="2">
         <v>50</v>
       </c>
       <c r="B51" s="2" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="52" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J51" s="2"/>
+      <c r="K51" s="2"/>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A52" s="2">
         <v>51</v>
       </c>
       <c r="B52" s="2" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="53" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J52" s="2"/>
+      <c r="K52" s="2"/>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A53" s="2">
         <v>52</v>
       </c>
       <c r="B53" s="2" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="54" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J53" s="2"/>
+      <c r="K53" s="2"/>
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A54" s="2">
         <v>53</v>
       </c>
       <c r="B54" s="2" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="55" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J54" s="2"/>
+      <c r="K54" s="2"/>
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A55" s="2">
         <v>54</v>
       </c>
       <c r="B55" s="2" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="56" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J55" s="2"/>
+      <c r="K55" s="2"/>
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A56" s="2">
         <v>55</v>
       </c>
       <c r="B56" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="57" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J56" s="2"/>
+      <c r="K56" s="2"/>
+    </row>
+    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A57" s="2">
         <v>56</v>
       </c>
       <c r="B57" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="58" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J57" s="2"/>
+      <c r="K57" s="2"/>
+    </row>
+    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A58" s="2">
         <v>57</v>
       </c>
       <c r="B58" s="2" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="59" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J58" s="2"/>
+      <c r="K58" s="2"/>
+    </row>
+    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A59" s="2">
         <v>58</v>
       </c>
       <c r="B59" s="2" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="60" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J59" s="2"/>
+      <c r="K59" s="2"/>
+    </row>
+    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A60" s="2">
         <v>59</v>
       </c>
       <c r="B60" s="2" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J60" s="2"/>
+      <c r="K60" s="2"/>
+    </row>
+    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A61" s="2">
         <v>60</v>
       </c>
@@ -2598,11 +2758,13 @@
       <c r="G61" s="2" t="s">
         <v>369</v>
       </c>
-      <c r="I61" s="2" t="s">
+      <c r="J61" s="2"/>
+      <c r="K61" s="2"/>
+      <c r="L61" s="2" t="s">
         <v>371</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A62" s="2">
         <v>60</v>
       </c>
@@ -2624,19 +2786,23 @@
       <c r="G62" s="2" t="s">
         <v>370</v>
       </c>
-      <c r="I62" s="2" t="s">
+      <c r="J62" s="2"/>
+      <c r="K62" s="2"/>
+      <c r="L62" s="2" t="s">
         <v>372</v>
       </c>
     </row>
-    <row r="63" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A63" s="2">
         <v>61</v>
       </c>
       <c r="B63" s="2" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J63" s="2"/>
+      <c r="K63" s="2"/>
+    </row>
+    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A64" s="2">
         <v>62</v>
       </c>
@@ -2658,11 +2824,13 @@
       <c r="G64" s="2" t="s">
         <v>363</v>
       </c>
-      <c r="I64" s="2" t="s">
+      <c r="J64" s="2"/>
+      <c r="K64" s="2"/>
+      <c r="L64" s="2" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A65" s="2">
         <v>63</v>
       </c>
@@ -2684,11 +2852,13 @@
       <c r="G65" s="2" t="s">
         <v>369</v>
       </c>
-      <c r="I65" s="2" t="s">
+      <c r="J65" s="2"/>
+      <c r="K65" s="2"/>
+      <c r="L65" s="2" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A66" s="2">
         <v>64</v>
       </c>
@@ -2707,11 +2877,13 @@
       <c r="F66" s="2" t="s">
         <v>377</v>
       </c>
-      <c r="I66" s="2" t="s">
+      <c r="J66" s="2"/>
+      <c r="K66" s="2"/>
+      <c r="L66" s="2" t="s">
         <v>378</v>
       </c>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A67" s="2">
         <v>65</v>
       </c>
@@ -2733,11 +2905,13 @@
       <c r="G67" s="2" t="s">
         <v>363</v>
       </c>
-      <c r="I67" s="2" t="s">
+      <c r="J67" s="2"/>
+      <c r="K67" s="2"/>
+      <c r="L67" s="2" t="s">
         <v>355</v>
       </c>
     </row>
-    <row r="68" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A68" s="3">
         <v>65</v>
       </c>
@@ -2760,19 +2934,23 @@
         <v>363</v>
       </c>
       <c r="H68" s="3"/>
-      <c r="I68" s="3" t="s">
+      <c r="J68" s="3"/>
+      <c r="K68" s="3"/>
+      <c r="L68" s="3" t="s">
         <v>355</v>
       </c>
     </row>
-    <row r="69" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A69" s="2">
         <v>66</v>
       </c>
       <c r="B69" s="2" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J69" s="2"/>
+      <c r="K69" s="2"/>
+    </row>
+    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A70" s="4">
         <v>67</v>
       </c>
@@ -2797,11 +2975,13 @@
       <c r="H70" s="4" t="s">
         <v>514</v>
       </c>
-      <c r="I70" s="4" t="s">
+      <c r="J70" s="2"/>
+      <c r="K70" s="2"/>
+      <c r="L70" s="4" t="s">
         <v>359</v>
       </c>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A71" s="2">
         <v>67</v>
       </c>
@@ -2826,11 +3006,13 @@
       <c r="H71" s="2" t="s">
         <v>503</v>
       </c>
-      <c r="I71" s="2" t="s">
+      <c r="J71" s="2"/>
+      <c r="K71" s="2"/>
+      <c r="L71" s="2" t="s">
         <v>387</v>
       </c>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A72" s="2">
         <v>68</v>
       </c>
@@ -2852,35 +3034,43 @@
       <c r="G72" s="2" t="s">
         <v>363</v>
       </c>
-      <c r="I72" s="2" t="s">
+      <c r="J72" s="2"/>
+      <c r="K72" s="2"/>
+      <c r="L72" s="2" t="s">
         <v>355</v>
       </c>
     </row>
-    <row r="73" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A73" s="2">
         <v>69</v>
       </c>
       <c r="B73" s="2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="74" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J73" s="2"/>
+      <c r="K73" s="2"/>
+    </row>
+    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A74" s="2">
         <v>70</v>
       </c>
       <c r="B74" s="2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="75" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J74" s="2"/>
+      <c r="K74" s="2"/>
+    </row>
+    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A75" s="2">
         <v>71</v>
       </c>
       <c r="B75" s="2" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J75" s="2"/>
+      <c r="K75" s="2"/>
+    </row>
+    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A76" s="2">
         <v>72</v>
       </c>
@@ -2899,11 +3089,13 @@
       <c r="F76" s="2" t="s">
         <v>354</v>
       </c>
-      <c r="I76" s="2" t="s">
+      <c r="J76" s="2"/>
+      <c r="K76" s="2"/>
+      <c r="L76" s="2" t="s">
         <v>355</v>
       </c>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A77" s="2">
         <v>72</v>
       </c>
@@ -2922,19 +3114,23 @@
       <c r="F77" s="2" t="s">
         <v>358</v>
       </c>
-      <c r="I77" s="2" t="s">
+      <c r="J77" s="2"/>
+      <c r="K77" s="2"/>
+      <c r="L77" s="2" t="s">
         <v>359</v>
       </c>
     </row>
-    <row r="78" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A78" s="2">
         <v>73</v>
       </c>
       <c r="B78" s="2" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J78" s="2"/>
+      <c r="K78" s="2"/>
+    </row>
+    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A79" s="2">
         <v>74</v>
       </c>
@@ -2956,11 +3152,13 @@
       <c r="G79" s="2" t="s">
         <v>363</v>
       </c>
-      <c r="I79" s="2" t="s">
+      <c r="J79" s="2"/>
+      <c r="K79" s="2"/>
+      <c r="L79" s="2" t="s">
         <v>359</v>
       </c>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A80" s="2">
         <v>74</v>
       </c>
@@ -2982,11 +3180,13 @@
       <c r="G80" s="2" t="s">
         <v>399</v>
       </c>
-      <c r="I80" s="2" t="s">
+      <c r="J80" s="2"/>
+      <c r="K80" s="2"/>
+      <c r="L80" s="2" t="s">
         <v>400</v>
       </c>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A81" s="2">
         <v>74</v>
       </c>
@@ -3011,11 +3211,13 @@
       <c r="H81" s="2" t="s">
         <v>455</v>
       </c>
-      <c r="I81" s="2" t="s">
+      <c r="J81" s="2"/>
+      <c r="K81" s="2"/>
+      <c r="L81" s="2" t="s">
         <v>359</v>
       </c>
     </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A82" s="2">
         <v>75</v>
       </c>
@@ -3037,43 +3239,53 @@
       <c r="G82" s="2" t="s">
         <v>392</v>
       </c>
-      <c r="I82" s="2" t="s">
+      <c r="J82" s="2"/>
+      <c r="K82" s="2"/>
+      <c r="L82" s="2" t="s">
         <v>393</v>
       </c>
     </row>
-    <row r="83" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A83" s="2">
         <v>76</v>
       </c>
       <c r="B83" s="2" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="84" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J83" s="2"/>
+      <c r="K83" s="2"/>
+    </row>
+    <row r="84" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A84" s="2">
         <v>77</v>
       </c>
       <c r="B84" s="2" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="85" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J84" s="2"/>
+      <c r="K84" s="2"/>
+    </row>
+    <row r="85" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A85" s="2">
         <v>78</v>
       </c>
       <c r="B85" s="2" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="86" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J85" s="2"/>
+      <c r="K85" s="2"/>
+    </row>
+    <row r="86" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A86" s="2">
         <v>79</v>
       </c>
       <c r="B86" s="2" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J86" s="2"/>
+      <c r="K86" s="2"/>
+    </row>
+    <row r="87" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A87" s="2">
         <v>80</v>
       </c>
@@ -3095,83 +3307,103 @@
       <c r="G87" s="2" t="s">
         <v>363</v>
       </c>
-      <c r="I87" s="2" t="s">
+      <c r="J87" s="2"/>
+      <c r="K87" s="2"/>
+      <c r="L87" s="2" t="s">
         <v>406</v>
       </c>
     </row>
-    <row r="88" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A88" s="2">
         <v>81</v>
       </c>
       <c r="B88" s="2" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="89" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J88" s="2"/>
+      <c r="K88" s="2"/>
+    </row>
+    <row r="89" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A89" s="2">
         <v>82</v>
       </c>
       <c r="B89" s="2" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="90" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J89" s="2"/>
+      <c r="K89" s="2"/>
+    </row>
+    <row r="90" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A90" s="2">
         <v>83</v>
       </c>
       <c r="B90" s="2" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="91" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J90" s="2"/>
+      <c r="K90" s="2"/>
+    </row>
+    <row r="91" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A91" s="2">
         <v>84</v>
       </c>
       <c r="B91" s="2" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="92" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J91" s="2"/>
+      <c r="K91" s="2"/>
+    </row>
+    <row r="92" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A92" s="2">
         <v>85</v>
       </c>
       <c r="B92" s="2" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="93" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J92" s="2"/>
+      <c r="K92" s="2"/>
+    </row>
+    <row r="93" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A93" s="2">
         <v>86</v>
       </c>
       <c r="B93" s="2" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="94" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J93" s="2"/>
+      <c r="K93" s="2"/>
+    </row>
+    <row r="94" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A94" s="2">
         <v>87</v>
       </c>
       <c r="B94" s="2" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="95" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J94" s="2"/>
+      <c r="K94" s="2"/>
+    </row>
+    <row r="95" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A95" s="2">
         <v>88</v>
       </c>
       <c r="B95" s="2" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="96" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J95" s="2"/>
+      <c r="K95" s="2"/>
+    </row>
+    <row r="96" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A96" s="2">
         <v>89</v>
       </c>
       <c r="B96" s="2" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J96" s="2"/>
+      <c r="K96" s="2"/>
+    </row>
+    <row r="97" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A97" s="2">
         <v>90</v>
       </c>
@@ -3193,11 +3425,13 @@
       <c r="G97" s="2" t="s">
         <v>363</v>
       </c>
-      <c r="I97" s="2" t="s">
+      <c r="J97" s="2"/>
+      <c r="K97" s="2"/>
+      <c r="L97" s="2" t="s">
         <v>413</v>
       </c>
     </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A98" s="2">
         <v>91</v>
       </c>
@@ -3219,11 +3453,13 @@
       <c r="G98" s="2" t="s">
         <v>412</v>
       </c>
-      <c r="I98" s="2" t="s">
+      <c r="J98" s="2"/>
+      <c r="K98" s="2"/>
+      <c r="L98" s="2" t="s">
         <v>413</v>
       </c>
     </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A99" s="2">
         <v>91</v>
       </c>
@@ -3245,11 +3481,13 @@
       <c r="H99" s="2" t="s">
         <v>504</v>
       </c>
-      <c r="I99" s="2" t="s">
+      <c r="J99" s="2"/>
+      <c r="K99" s="2"/>
+      <c r="L99" s="2" t="s">
         <v>413</v>
       </c>
     </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A100" s="2">
         <v>92</v>
       </c>
@@ -3271,11 +3509,13 @@
       <c r="H100" s="2" t="s">
         <v>515</v>
       </c>
-      <c r="I100" s="2" t="s">
+      <c r="J100" s="2"/>
+      <c r="K100" s="2"/>
+      <c r="L100" s="2" t="s">
         <v>415</v>
       </c>
     </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A101" s="2">
         <v>93</v>
       </c>
@@ -3297,11 +3537,13 @@
       <c r="G101" s="2" t="s">
         <v>363</v>
       </c>
-      <c r="I101" s="2" t="s">
+      <c r="J101" s="2"/>
+      <c r="K101" s="2"/>
+      <c r="L101" s="2" t="s">
         <v>355</v>
       </c>
     </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A102" s="2">
         <v>94</v>
       </c>
@@ -3326,27 +3568,33 @@
       <c r="H102" s="2" t="s">
         <v>507</v>
       </c>
-      <c r="I102" s="2" t="s">
+      <c r="J102" s="2"/>
+      <c r="K102" s="2"/>
+      <c r="L102" s="2" t="s">
         <v>413</v>
       </c>
     </row>
-    <row r="103" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A103" s="2">
         <v>95</v>
       </c>
       <c r="B103" s="2" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="104" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J103" s="2"/>
+      <c r="K103" s="2"/>
+    </row>
+    <row r="104" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A104" s="2">
         <v>96</v>
       </c>
       <c r="B104" s="2" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J104" s="2"/>
+      <c r="K104" s="2"/>
+    </row>
+    <row r="105" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A105" s="2">
         <v>97</v>
       </c>
@@ -3368,11 +3616,13 @@
       <c r="G105" s="2" t="s">
         <v>363</v>
       </c>
-      <c r="I105" s="2" t="s">
+      <c r="J105" s="2"/>
+      <c r="K105" s="2"/>
+      <c r="L105" s="2" t="s">
         <v>427</v>
       </c>
     </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A106" s="2">
         <v>98</v>
       </c>
@@ -3397,11 +3647,13 @@
       <c r="H106" s="2" t="s">
         <v>519</v>
       </c>
-      <c r="I106" s="2" t="s">
+      <c r="J106" s="2"/>
+      <c r="K106" s="2"/>
+      <c r="L106" s="2" t="s">
         <v>436</v>
       </c>
     </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A107" s="2">
         <v>99</v>
       </c>
@@ -3426,11 +3678,13 @@
       <c r="H107" s="2" t="s">
         <v>505</v>
       </c>
-      <c r="I107" s="2" t="s">
+      <c r="J107" s="2"/>
+      <c r="K107" s="2"/>
+      <c r="L107" s="2" t="s">
         <v>436</v>
       </c>
     </row>
-    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A108" s="2">
         <v>100</v>
       </c>
@@ -3452,11 +3706,13 @@
       <c r="H108" s="2" t="s">
         <v>506</v>
       </c>
-      <c r="I108" s="2" t="s">
+      <c r="J108" s="2"/>
+      <c r="K108" s="2"/>
+      <c r="L108" s="2" t="s">
         <v>431</v>
       </c>
     </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A109" s="5">
         <v>100</v>
       </c>
@@ -3477,43 +3733,53 @@
       </c>
       <c r="G109" s="5"/>
       <c r="H109" s="5"/>
-      <c r="I109" s="5" t="s">
+      <c r="J109" s="2"/>
+      <c r="K109" s="2"/>
+      <c r="L109" s="5" t="s">
         <v>427</v>
       </c>
     </row>
-    <row r="110" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A110" s="2">
         <v>101</v>
       </c>
       <c r="B110" s="2" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="111" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J110" s="2"/>
+      <c r="K110" s="2"/>
+    </row>
+    <row r="111" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A111" s="2">
         <v>102</v>
       </c>
       <c r="B111" s="2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="112" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J111" s="2"/>
+      <c r="K111" s="2"/>
+    </row>
+    <row r="112" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A112" s="2">
         <v>103</v>
       </c>
       <c r="B112" s="2" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="113" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J112" s="2"/>
+      <c r="K112" s="2"/>
+    </row>
+    <row r="113" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A113" s="2">
         <v>104</v>
       </c>
       <c r="B113" s="2" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="114" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J113" s="2"/>
+      <c r="K113" s="2"/>
+    </row>
+    <row r="114" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A114" s="2">
         <v>104</v>
       </c>
@@ -3535,19 +3801,23 @@
       <c r="G114" s="2" t="s">
         <v>363</v>
       </c>
-      <c r="I114" s="2" t="s">
+      <c r="J114" s="2"/>
+      <c r="K114" s="2"/>
+      <c r="L114" s="2" t="s">
         <v>427</v>
       </c>
     </row>
-    <row r="115" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A115" s="2">
         <v>105</v>
       </c>
       <c r="B115" s="2" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="116" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J115" s="2"/>
+      <c r="K115" s="2"/>
+    </row>
+    <row r="116" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A116" s="2">
         <v>105</v>
       </c>
@@ -3569,67 +3839,83 @@
       <c r="G116" s="2" t="s">
         <v>363</v>
       </c>
-      <c r="I116" s="2" t="s">
+      <c r="J116" s="2"/>
+      <c r="K116" s="2"/>
+      <c r="L116" s="2" t="s">
         <v>413</v>
       </c>
     </row>
-    <row r="117" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A117" s="2">
         <v>106</v>
       </c>
       <c r="B117" s="2" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="118" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J117" s="2"/>
+      <c r="K117" s="2"/>
+    </row>
+    <row r="118" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A118" s="2">
         <v>107</v>
       </c>
       <c r="B118" s="2" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="119" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J118" s="2"/>
+      <c r="K118" s="2"/>
+    </row>
+    <row r="119" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A119" s="2">
         <v>108</v>
       </c>
       <c r="B119" s="2" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="120" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J119" s="2"/>
+      <c r="K119" s="2"/>
+    </row>
+    <row r="120" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A120" s="2">
         <v>109</v>
       </c>
       <c r="B120" s="2" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="121" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J120" s="2"/>
+      <c r="K120" s="2"/>
+    </row>
+    <row r="121" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A121" s="2">
         <v>110</v>
       </c>
       <c r="B121" s="2" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="122" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J121" s="2"/>
+      <c r="K121" s="2"/>
+    </row>
+    <row r="122" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A122" s="2">
         <v>111</v>
       </c>
       <c r="B122" s="2" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="123" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J122" s="2"/>
+      <c r="K122" s="2"/>
+    </row>
+    <row r="123" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A123" s="2">
         <v>112</v>
       </c>
       <c r="B123" s="2" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="124" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J123" s="2"/>
+      <c r="K123" s="2"/>
+    </row>
+    <row r="124" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A124" s="2">
         <v>113</v>
       </c>
@@ -3654,11 +3940,13 @@
       <c r="H124" s="2" t="s">
         <v>510</v>
       </c>
-      <c r="I124" s="2" t="s">
+      <c r="J124" s="2"/>
+      <c r="K124" s="2"/>
+      <c r="L124" s="2" t="s">
         <v>443</v>
       </c>
     </row>
-    <row r="125" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A125" s="2">
         <v>114</v>
       </c>
@@ -3680,83 +3968,103 @@
       <c r="G125" s="2" t="s">
         <v>369</v>
       </c>
-      <c r="I125" s="2" t="s">
+      <c r="J125" s="2"/>
+      <c r="K125" s="2"/>
+      <c r="L125" s="2" t="s">
         <v>443</v>
       </c>
     </row>
-    <row r="126" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A126" s="2">
         <v>115</v>
       </c>
       <c r="B126" s="2" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="127" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J126" s="2"/>
+      <c r="K126" s="2"/>
+    </row>
+    <row r="127" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A127" s="2">
         <v>116</v>
       </c>
       <c r="B127" s="2" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="128" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J127" s="2"/>
+      <c r="K127" s="2"/>
+    </row>
+    <row r="128" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A128" s="2">
         <v>117</v>
       </c>
       <c r="B128" s="2" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="129" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J128" s="2"/>
+      <c r="K128" s="2"/>
+    </row>
+    <row r="129" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A129" s="2">
         <v>118</v>
       </c>
       <c r="B129" s="2" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="130" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J129" s="2"/>
+      <c r="K129" s="2"/>
+    </row>
+    <row r="130" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A130" s="2">
         <v>119</v>
       </c>
       <c r="B130" s="2" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="131" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J130" s="2"/>
+      <c r="K130" s="2"/>
+    </row>
+    <row r="131" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A131" s="2">
         <v>120</v>
       </c>
       <c r="B131" s="2" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="132" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J131" s="2"/>
+      <c r="K131" s="2"/>
+    </row>
+    <row r="132" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A132" s="2">
         <v>121</v>
       </c>
       <c r="B132" s="2" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="133" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J132" s="2"/>
+      <c r="K132" s="2"/>
+    </row>
+    <row r="133" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A133" s="2">
         <v>122</v>
       </c>
       <c r="B133" s="2" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="134" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J133" s="2"/>
+      <c r="K133" s="2"/>
+    </row>
+    <row r="134" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A134" s="2">
         <v>123</v>
       </c>
       <c r="B134" s="2" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="135" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J134" s="2"/>
+      <c r="K134" s="2"/>
+    </row>
+    <row r="135" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A135" s="5">
         <v>124</v>
       </c>
@@ -3779,11 +4087,13 @@
       <c r="H135" s="5" t="s">
         <v>522</v>
       </c>
-      <c r="I135" s="5" t="s">
+      <c r="J135" s="2"/>
+      <c r="K135" s="2"/>
+      <c r="L135" s="5" t="s">
         <v>523</v>
       </c>
     </row>
-    <row r="136" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A136" s="2">
         <v>125</v>
       </c>
@@ -3805,67 +4115,83 @@
       <c r="G136" s="2" t="s">
         <v>369</v>
       </c>
-      <c r="I136" s="2" t="s">
+      <c r="J136" s="2"/>
+      <c r="K136" s="2"/>
+      <c r="L136" s="2" t="s">
         <v>449</v>
       </c>
     </row>
-    <row r="137" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A137" s="2">
         <v>126</v>
       </c>
       <c r="B137" s="2" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="138" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J137" s="2"/>
+      <c r="K137" s="2"/>
+    </row>
+    <row r="138" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A138" s="2">
         <v>127</v>
       </c>
       <c r="B138" s="2" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="139" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J138" s="2"/>
+      <c r="K138" s="2"/>
+    </row>
+    <row r="139" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A139" s="2">
         <v>128</v>
       </c>
       <c r="B139" s="2" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="140" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J139" s="2"/>
+      <c r="K139" s="2"/>
+    </row>
+    <row r="140" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A140" s="2">
         <v>129</v>
       </c>
       <c r="B140" s="2" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="141" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J140" s="2"/>
+      <c r="K140" s="2"/>
+    </row>
+    <row r="141" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A141" s="2">
         <v>130</v>
       </c>
       <c r="B141" s="2" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="142" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J141" s="2"/>
+      <c r="K141" s="2"/>
+    </row>
+    <row r="142" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A142" s="2">
         <v>131</v>
       </c>
       <c r="B142" s="2" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="143" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J142" s="2"/>
+      <c r="K142" s="2"/>
+    </row>
+    <row r="143" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A143" s="2">
         <v>132</v>
       </c>
       <c r="B143" s="2" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="144" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J143" s="2"/>
+      <c r="K143" s="2"/>
+    </row>
+    <row r="144" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A144" s="2">
         <v>133</v>
       </c>
@@ -3887,67 +4213,83 @@
       <c r="G144" s="2" t="s">
         <v>369</v>
       </c>
-      <c r="I144" s="2" t="s">
+      <c r="J144" s="2"/>
+      <c r="K144" s="2"/>
+      <c r="L144" s="2" t="s">
         <v>371</v>
       </c>
     </row>
-    <row r="145" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A145" s="2">
         <v>134</v>
       </c>
       <c r="B145" s="2" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="146" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J145" s="2"/>
+      <c r="K145" s="2"/>
+    </row>
+    <row r="146" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A146" s="2">
         <v>135</v>
       </c>
       <c r="B146" s="2" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="147" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J146" s="2"/>
+      <c r="K146" s="2"/>
+    </row>
+    <row r="147" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A147" s="2">
         <v>136</v>
       </c>
       <c r="B147" s="2" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="148" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J147" s="2"/>
+      <c r="K147" s="2"/>
+    </row>
+    <row r="148" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A148" s="2">
         <v>137</v>
       </c>
       <c r="B148" s="2" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="149" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J148" s="2"/>
+      <c r="K148" s="2"/>
+    </row>
+    <row r="149" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A149" s="2">
         <v>138</v>
       </c>
       <c r="B149" s="2" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="150" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J149" s="2"/>
+      <c r="K149" s="2"/>
+    </row>
+    <row r="150" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A150" s="2">
         <v>139</v>
       </c>
       <c r="B150" s="2" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="151" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J150" s="2"/>
+      <c r="K150" s="2"/>
+    </row>
+    <row r="151" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A151" s="2">
         <v>140</v>
       </c>
       <c r="B151" s="2" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="152" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J151" s="2"/>
+      <c r="K151" s="2"/>
+    </row>
+    <row r="152" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A152" s="2">
         <v>141</v>
       </c>
@@ -3969,11 +4311,13 @@
       <c r="G152" s="2" t="s">
         <v>369</v>
       </c>
-      <c r="I152" s="2" t="s">
+      <c r="J152" s="2"/>
+      <c r="K152" s="2"/>
+      <c r="L152" s="2" t="s">
         <v>371</v>
       </c>
     </row>
-    <row r="153" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A153" s="2">
         <v>142</v>
       </c>
@@ -3998,11 +4342,13 @@
       <c r="H153" s="2" t="s">
         <v>511</v>
       </c>
-      <c r="I153" s="2" t="s">
+      <c r="J153" s="2"/>
+      <c r="K153" s="2"/>
+      <c r="L153" s="2" t="s">
         <v>431</v>
       </c>
     </row>
-    <row r="154" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A154" s="2">
         <v>142</v>
       </c>
@@ -4024,43 +4370,53 @@
       <c r="G154" s="2" t="s">
         <v>363</v>
       </c>
-      <c r="I154" s="2" t="s">
+      <c r="J154" s="2"/>
+      <c r="K154" s="2"/>
+      <c r="L154" s="2" t="s">
         <v>431</v>
       </c>
     </row>
-    <row r="155" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A155" s="2">
         <v>143</v>
       </c>
       <c r="B155" s="2" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="156" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J155" s="2"/>
+      <c r="K155" s="2"/>
+    </row>
+    <row r="156" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A156" s="2">
         <v>144</v>
       </c>
       <c r="B156" s="2" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="157" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J156" s="2"/>
+      <c r="K156" s="2"/>
+    </row>
+    <row r="157" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A157" s="2">
         <v>145</v>
       </c>
       <c r="B157" s="2" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="158" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J157" s="2"/>
+      <c r="K157" s="2"/>
+    </row>
+    <row r="158" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A158" s="2">
         <v>146</v>
       </c>
       <c r="B158" s="2" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="159" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J158" s="2"/>
+      <c r="K158" s="2"/>
+    </row>
+    <row r="159" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A159" s="2">
         <v>147</v>
       </c>
@@ -4082,11 +4438,13 @@
       <c r="H159" s="2" t="s">
         <v>467</v>
       </c>
-      <c r="I159" s="2" t="s">
+      <c r="J159" s="2"/>
+      <c r="K159" s="2"/>
+      <c r="L159" s="2" t="s">
         <v>431</v>
       </c>
     </row>
-    <row r="160" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A160" s="2">
         <v>147</v>
       </c>
@@ -4108,11 +4466,13 @@
       <c r="G160" s="2" t="s">
         <v>363</v>
       </c>
-      <c r="I160" s="2" t="s">
+      <c r="J160" s="2"/>
+      <c r="K160" s="2"/>
+      <c r="L160" s="2" t="s">
         <v>431</v>
       </c>
     </row>
-    <row r="161" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A161" s="5">
         <v>148</v>
       </c>
@@ -4135,35 +4495,43 @@
         <v>464</v>
       </c>
       <c r="H161" s="5"/>
-      <c r="I161" s="5" t="s">
+      <c r="J161" s="5"/>
+      <c r="K161" s="5"/>
+      <c r="L161" s="5" t="s">
         <v>351</v>
       </c>
     </row>
-    <row r="162" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A162" s="2">
         <v>149</v>
       </c>
       <c r="B162" s="2" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="163" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J162" s="2"/>
+      <c r="K162" s="2"/>
+    </row>
+    <row r="163" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A163" s="2">
         <v>150</v>
       </c>
       <c r="B163" s="2" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="164" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J163" s="2"/>
+      <c r="K163" s="2"/>
+    </row>
+    <row r="164" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A164" s="2">
         <v>151</v>
       </c>
       <c r="B164" s="2" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="165" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J164" s="2"/>
+      <c r="K164" s="2"/>
+    </row>
+    <row r="165" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A165" s="2">
         <v>152</v>
       </c>
@@ -4185,291 +4553,363 @@
       <c r="H165" s="2" t="s">
         <v>455</v>
       </c>
-      <c r="I165" s="2" t="s">
+      <c r="J165" s="2"/>
+      <c r="K165" s="2"/>
+      <c r="L165" s="2" t="s">
         <v>456</v>
       </c>
     </row>
-    <row r="166" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A166" s="2">
         <v>153</v>
       </c>
       <c r="B166" s="2" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="167" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J166" s="2"/>
+      <c r="K166" s="2"/>
+    </row>
+    <row r="167" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A167" s="2">
         <v>154</v>
       </c>
       <c r="B167" s="2" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="168" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J167" s="2"/>
+      <c r="K167" s="2"/>
+    </row>
+    <row r="168" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A168" s="2">
         <v>155</v>
       </c>
       <c r="B168" s="2" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="169" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J168" s="2"/>
+      <c r="K168" s="2"/>
+    </row>
+    <row r="169" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A169" s="2">
         <v>156</v>
       </c>
       <c r="B169" s="2" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="170" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J169" s="2"/>
+      <c r="K169" s="2"/>
+    </row>
+    <row r="170" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A170" s="2">
         <v>157</v>
       </c>
       <c r="B170" s="2" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="171" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J170" s="2"/>
+      <c r="K170" s="2"/>
+    </row>
+    <row r="171" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A171" s="2">
         <v>158</v>
       </c>
       <c r="B171" s="2" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="172" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J171" s="2"/>
+      <c r="K171" s="2"/>
+    </row>
+    <row r="172" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A172" s="2">
         <v>159</v>
       </c>
       <c r="B172" s="2" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="173" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J172" s="2"/>
+      <c r="K172" s="2"/>
+    </row>
+    <row r="173" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A173" s="2">
         <v>160</v>
       </c>
       <c r="B173" s="2" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="174" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J173" s="2"/>
+      <c r="K173" s="2"/>
+    </row>
+    <row r="174" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A174" s="2">
         <v>161</v>
       </c>
       <c r="B174" s="2" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="175" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J174" s="2"/>
+      <c r="K174" s="2"/>
+    </row>
+    <row r="175" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A175" s="2">
         <v>162</v>
       </c>
       <c r="B175" s="2" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="176" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J175" s="2"/>
+      <c r="K175" s="2"/>
+    </row>
+    <row r="176" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A176" s="2">
         <v>163</v>
       </c>
       <c r="B176" s="2" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="177" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J176" s="2"/>
+      <c r="K176" s="2"/>
+    </row>
+    <row r="177" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A177" s="2">
         <v>164</v>
       </c>
       <c r="B177" s="2" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="178" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J177" s="2"/>
+      <c r="K177" s="2"/>
+    </row>
+    <row r="178" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A178" s="2">
         <v>165</v>
       </c>
       <c r="B178" s="2" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="179" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J178" s="2"/>
+      <c r="K178" s="2"/>
+    </row>
+    <row r="179" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A179" s="2">
         <v>166</v>
       </c>
       <c r="B179" s="2" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="180" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J179" s="2"/>
+      <c r="K179" s="2"/>
+    </row>
+    <row r="180" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A180" s="2">
         <v>167</v>
       </c>
       <c r="B180" s="2" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="181" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J180" s="2"/>
+      <c r="K180" s="2"/>
+    </row>
+    <row r="181" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A181" s="2">
         <v>168</v>
       </c>
       <c r="B181" s="2" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="182" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J181" s="2"/>
+      <c r="K181" s="2"/>
+    </row>
+    <row r="182" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A182" s="2">
         <v>169</v>
       </c>
       <c r="B182" s="2" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="183" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J182" s="2"/>
+      <c r="K182" s="2"/>
+    </row>
+    <row r="183" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A183" s="2">
         <v>170</v>
       </c>
       <c r="B183" s="2" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="184" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J183" s="2"/>
+      <c r="K183" s="2"/>
+    </row>
+    <row r="184" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A184" s="2">
         <v>171</v>
       </c>
       <c r="B184" s="2" t="s">
         <v>179</v>
       </c>
-    </row>
-    <row r="185" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J184" s="2"/>
+      <c r="K184" s="2"/>
+    </row>
+    <row r="185" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A185" s="2">
         <v>172</v>
       </c>
       <c r="B185" s="2" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="186" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J185" s="2"/>
+      <c r="K185" s="2"/>
+    </row>
+    <row r="186" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A186" s="2">
         <v>173</v>
       </c>
       <c r="B186" s="2" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="187" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J186" s="2"/>
+      <c r="K186" s="2"/>
+    </row>
+    <row r="187" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A187" s="2">
         <v>174</v>
       </c>
       <c r="B187" s="2" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="188" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J187" s="2"/>
+      <c r="K187" s="2"/>
+    </row>
+    <row r="188" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A188" s="2">
         <v>175</v>
       </c>
       <c r="B188" s="2" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="189" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J188" s="2"/>
+      <c r="K188" s="2"/>
+    </row>
+    <row r="189" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A189" s="2">
         <v>176</v>
       </c>
       <c r="B189" s="2" t="s">
         <v>184</v>
       </c>
-    </row>
-    <row r="190" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J189" s="2"/>
+      <c r="K189" s="2"/>
+    </row>
+    <row r="190" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A190" s="2">
         <v>177</v>
       </c>
       <c r="B190" s="2" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="191" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J190" s="2"/>
+      <c r="K190" s="2"/>
+    </row>
+    <row r="191" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A191" s="2">
         <v>178</v>
       </c>
       <c r="B191" s="2" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="192" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J191" s="2"/>
+      <c r="K191" s="2"/>
+    </row>
+    <row r="192" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A192" s="2">
         <v>179</v>
       </c>
       <c r="B192" s="2" t="s">
         <v>188</v>
       </c>
-    </row>
-    <row r="193" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J192" s="2"/>
+      <c r="K192" s="2"/>
+    </row>
+    <row r="193" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A193" s="2">
         <v>180</v>
       </c>
       <c r="B193" s="2" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="194" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J193" s="2"/>
+      <c r="K193" s="2"/>
+    </row>
+    <row r="194" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A194" s="2">
         <v>181</v>
       </c>
       <c r="B194" s="2" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="195" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J194" s="2"/>
+      <c r="K194" s="2"/>
+    </row>
+    <row r="195" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A195" s="2">
         <v>182</v>
       </c>
       <c r="B195" s="2" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="196" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J195" s="2"/>
+      <c r="K195" s="2"/>
+    </row>
+    <row r="196" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A196" s="2">
         <v>183</v>
       </c>
       <c r="B196" s="2" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="197" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J196" s="2"/>
+      <c r="K196" s="2"/>
+    </row>
+    <row r="197" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A197" s="2">
         <v>184</v>
       </c>
       <c r="B197" s="2" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="198" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J197" s="2"/>
+      <c r="K197" s="2"/>
+    </row>
+    <row r="198" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A198" s="2">
         <v>185</v>
       </c>
       <c r="B198" s="2" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="199" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J198" s="2"/>
+      <c r="K198" s="2"/>
+    </row>
+    <row r="199" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A199" s="2">
         <v>186</v>
       </c>
       <c r="B199" s="2" t="s">
         <v>198</v>
       </c>
-    </row>
-    <row r="200" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J199" s="2"/>
+      <c r="K199" s="2"/>
+    </row>
+    <row r="200" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A200" s="2">
         <v>187</v>
       </c>
       <c r="B200" s="2" t="s">
         <v>194</v>
       </c>
-    </row>
-    <row r="201" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J200" s="2"/>
+      <c r="K200" s="2"/>
+    </row>
+    <row r="201" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A201" s="2">
         <v>188</v>
       </c>
@@ -4491,11 +4931,13 @@
       <c r="H201" s="2" t="s">
         <v>512</v>
       </c>
-      <c r="I201" s="2" t="s">
+      <c r="J201" s="2"/>
+      <c r="K201" s="2"/>
+      <c r="L201" s="2" t="s">
         <v>427</v>
       </c>
     </row>
-    <row r="202" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A202" s="2">
         <v>188</v>
       </c>
@@ -4517,99 +4959,123 @@
       <c r="G202" s="2" t="s">
         <v>363</v>
       </c>
-      <c r="I202" s="2" t="s">
+      <c r="J202" s="2"/>
+      <c r="K202" s="2"/>
+      <c r="L202" s="2" t="s">
         <v>427</v>
       </c>
     </row>
-    <row r="203" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A203" s="2">
         <v>189</v>
       </c>
       <c r="B203" s="2" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="204" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J203" s="2"/>
+      <c r="K203" s="2"/>
+    </row>
+    <row r="204" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A204" s="2">
         <v>190</v>
       </c>
       <c r="B204" s="2" t="s">
         <v>197</v>
       </c>
-    </row>
-    <row r="205" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J204" s="2"/>
+      <c r="K204" s="2"/>
+    </row>
+    <row r="205" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A205" s="2">
         <v>191</v>
       </c>
       <c r="B205" s="2" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="206" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J205" s="2"/>
+      <c r="K205" s="2"/>
+    </row>
+    <row r="206" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A206" s="2">
         <v>192</v>
       </c>
       <c r="B206" s="2" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="207" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J206" s="2"/>
+      <c r="K206" s="2"/>
+    </row>
+    <row r="207" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A207" s="2">
         <v>193</v>
       </c>
       <c r="B207" s="2" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="208" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J207" s="2"/>
+      <c r="K207" s="2"/>
+    </row>
+    <row r="208" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A208" s="2">
         <v>194</v>
       </c>
       <c r="B208" s="2" t="s">
         <v>204</v>
       </c>
-    </row>
-    <row r="209" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J208" s="2"/>
+      <c r="K208" s="2"/>
+    </row>
+    <row r="209" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A209" s="2">
         <v>195</v>
       </c>
       <c r="B209" s="2" t="s">
         <v>203</v>
       </c>
-    </row>
-    <row r="210" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J209" s="2"/>
+      <c r="K209" s="2"/>
+    </row>
+    <row r="210" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A210" s="2">
         <v>196</v>
       </c>
       <c r="B210" s="2" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="211" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J210" s="2"/>
+      <c r="K210" s="2"/>
+    </row>
+    <row r="211" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A211" s="2">
         <v>197</v>
       </c>
       <c r="B211" s="2" t="s">
         <v>206</v>
       </c>
-    </row>
-    <row r="212" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J211" s="2"/>
+      <c r="K211" s="2"/>
+    </row>
+    <row r="212" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A212" s="2">
         <v>198</v>
       </c>
       <c r="B212" s="2" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="213" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J212" s="2"/>
+      <c r="K212" s="2"/>
+    </row>
+    <row r="213" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A213" s="2">
         <v>199</v>
       </c>
       <c r="B213" s="2" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="214" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J213" s="2"/>
+      <c r="K213" s="2"/>
+    </row>
+    <row r="214" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A214" s="2">
         <v>200</v>
       </c>
@@ -4634,291 +5100,363 @@
       <c r="H214" s="2" t="s">
         <v>513</v>
       </c>
-      <c r="I214" s="2" t="s">
+      <c r="J214" s="2"/>
+      <c r="K214" s="2"/>
+      <c r="L214" s="2" t="s">
         <v>463</v>
       </c>
     </row>
-    <row r="215" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A215" s="2">
         <v>201</v>
       </c>
       <c r="B215" s="2" t="s">
         <v>211</v>
       </c>
-    </row>
-    <row r="216" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J215" s="2"/>
+      <c r="K215" s="2"/>
+    </row>
+    <row r="216" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A216" s="2">
         <v>202</v>
       </c>
       <c r="B216" s="2" t="s">
         <v>212</v>
       </c>
-    </row>
-    <row r="217" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J216" s="2"/>
+      <c r="K216" s="2"/>
+    </row>
+    <row r="217" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A217" s="2">
         <v>203</v>
       </c>
       <c r="B217" s="2" t="s">
         <v>210</v>
       </c>
-    </row>
-    <row r="218" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J217" s="2"/>
+      <c r="K217" s="2"/>
+    </row>
+    <row r="218" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A218" s="2">
         <v>204</v>
       </c>
       <c r="B218" s="2" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="219" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J218" s="2"/>
+      <c r="K218" s="2"/>
+    </row>
+    <row r="219" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A219" s="2">
         <v>205</v>
       </c>
       <c r="B219" s="2" t="s">
         <v>213</v>
       </c>
-    </row>
-    <row r="220" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J219" s="2"/>
+      <c r="K219" s="2"/>
+    </row>
+    <row r="220" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A220" s="2">
         <v>206</v>
       </c>
       <c r="B220" s="2" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="221" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J220" s="2"/>
+      <c r="K220" s="2"/>
+    </row>
+    <row r="221" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A221" s="2">
         <v>207</v>
       </c>
       <c r="B221" s="2" t="s">
         <v>215</v>
       </c>
-    </row>
-    <row r="222" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J221" s="2"/>
+      <c r="K221" s="2"/>
+    </row>
+    <row r="222" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A222" s="2">
         <v>208</v>
       </c>
       <c r="B222" s="2" t="s">
         <v>216</v>
       </c>
-    </row>
-    <row r="223" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J222" s="2"/>
+      <c r="K222" s="2"/>
+    </row>
+    <row r="223" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A223" s="2">
         <v>209</v>
       </c>
       <c r="B223" s="2" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="224" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J223" s="2"/>
+      <c r="K223" s="2"/>
+    </row>
+    <row r="224" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A224" s="2">
         <v>210</v>
       </c>
       <c r="B224" s="2" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="225" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J224" s="2"/>
+      <c r="K224" s="2"/>
+    </row>
+    <row r="225" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A225" s="2">
         <v>211</v>
       </c>
       <c r="B225" s="2" t="s">
         <v>219</v>
       </c>
-    </row>
-    <row r="226" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J225" s="2"/>
+      <c r="K225" s="2"/>
+    </row>
+    <row r="226" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A226" s="2">
         <v>212</v>
       </c>
       <c r="B226" s="2" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="227" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J226" s="2"/>
+      <c r="K226" s="2"/>
+    </row>
+    <row r="227" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A227" s="2">
         <v>213</v>
       </c>
       <c r="B227" s="2" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="228" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J227" s="2"/>
+      <c r="K227" s="2"/>
+    </row>
+    <row r="228" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A228" s="2">
         <v>214</v>
       </c>
       <c r="B228" s="2" t="s">
         <v>222</v>
       </c>
-    </row>
-    <row r="229" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J228" s="2"/>
+      <c r="K228" s="2"/>
+    </row>
+    <row r="229" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A229" s="2">
         <v>215</v>
       </c>
       <c r="B229" s="2" t="s">
         <v>223</v>
       </c>
-    </row>
-    <row r="230" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J229" s="2"/>
+      <c r="K229" s="2"/>
+    </row>
+    <row r="230" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A230" s="2">
         <v>216</v>
       </c>
       <c r="B230" s="2" t="s">
         <v>224</v>
       </c>
-    </row>
-    <row r="231" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J230" s="2"/>
+      <c r="K230" s="2"/>
+    </row>
+    <row r="231" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A231" s="2">
         <v>217</v>
       </c>
       <c r="B231" s="2" t="s">
         <v>225</v>
       </c>
-    </row>
-    <row r="232" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J231" s="2"/>
+      <c r="K231" s="2"/>
+    </row>
+    <row r="232" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A232" s="2">
         <v>218</v>
       </c>
       <c r="B232" s="2" t="s">
         <v>226</v>
       </c>
-    </row>
-    <row r="233" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J232" s="2"/>
+      <c r="K232" s="2"/>
+    </row>
+    <row r="233" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A233" s="2">
         <v>219</v>
       </c>
       <c r="B233" s="2" t="s">
         <v>227</v>
       </c>
-    </row>
-    <row r="234" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J233" s="2"/>
+      <c r="K233" s="2"/>
+    </row>
+    <row r="234" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A234" s="2">
         <v>220</v>
       </c>
       <c r="B234" s="2" t="s">
         <v>228</v>
       </c>
-    </row>
-    <row r="235" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J234" s="2"/>
+      <c r="K234" s="2"/>
+    </row>
+    <row r="235" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A235" s="2">
         <v>221</v>
       </c>
       <c r="B235" s="2" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="236" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J235" s="2"/>
+      <c r="K235" s="2"/>
+    </row>
+    <row r="236" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A236" s="2">
         <v>222</v>
       </c>
       <c r="B236" s="2" t="s">
         <v>230</v>
       </c>
-    </row>
-    <row r="237" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J236" s="2"/>
+      <c r="K236" s="2"/>
+    </row>
+    <row r="237" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A237" s="2">
         <v>223</v>
       </c>
       <c r="B237" s="2" t="s">
         <v>231</v>
       </c>
-    </row>
-    <row r="238" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J237" s="2"/>
+      <c r="K237" s="2"/>
+    </row>
+    <row r="238" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A238" s="2">
         <v>224</v>
       </c>
       <c r="B238" s="2" t="s">
         <v>233</v>
       </c>
-    </row>
-    <row r="239" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J238" s="2"/>
+      <c r="K238" s="2"/>
+    </row>
+    <row r="239" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A239" s="2">
         <v>225</v>
       </c>
       <c r="B239" s="2" t="s">
         <v>232</v>
       </c>
-    </row>
-    <row r="240" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J239" s="2"/>
+      <c r="K239" s="2"/>
+    </row>
+    <row r="240" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A240" s="2">
         <v>226</v>
       </c>
       <c r="B240" s="2" t="s">
         <v>234</v>
       </c>
-    </row>
-    <row r="241" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J240" s="2"/>
+      <c r="K240" s="2"/>
+    </row>
+    <row r="241" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A241" s="2">
         <v>227</v>
       </c>
       <c r="B241" s="2" t="s">
         <v>235</v>
       </c>
-    </row>
-    <row r="242" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J241" s="2"/>
+      <c r="K241" s="2"/>
+    </row>
+    <row r="242" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A242" s="2">
         <v>228</v>
       </c>
       <c r="B242" s="2" t="s">
         <v>236</v>
       </c>
-    </row>
-    <row r="243" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J242" s="2"/>
+      <c r="K242" s="2"/>
+    </row>
+    <row r="243" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A243" s="2">
         <v>229</v>
       </c>
       <c r="B243" s="2" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="244" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J243" s="2"/>
+      <c r="K243" s="2"/>
+    </row>
+    <row r="244" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A244" s="2">
         <v>230</v>
       </c>
       <c r="B244" s="2" t="s">
         <v>238</v>
       </c>
-    </row>
-    <row r="245" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J244" s="2"/>
+      <c r="K244" s="2"/>
+    </row>
+    <row r="245" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A245" s="2">
         <v>231</v>
       </c>
       <c r="B245" s="2" t="s">
         <v>239</v>
       </c>
-    </row>
-    <row r="246" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J245" s="2"/>
+      <c r="K245" s="2"/>
+    </row>
+    <row r="246" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A246" s="2">
         <v>232</v>
       </c>
       <c r="B246" s="2" t="s">
         <v>240</v>
       </c>
-    </row>
-    <row r="247" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J246" s="2"/>
+      <c r="K246" s="2"/>
+    </row>
+    <row r="247" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A247" s="2">
         <v>233</v>
       </c>
       <c r="B247" s="2" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="248" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J247" s="2"/>
+      <c r="K247" s="2"/>
+    </row>
+    <row r="248" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A248" s="2">
         <v>234</v>
       </c>
       <c r="B248" s="2" t="s">
         <v>242</v>
       </c>
-    </row>
-    <row r="249" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J248" s="2"/>
+      <c r="K248" s="2"/>
+    </row>
+    <row r="249" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A249" s="2">
         <v>235</v>
       </c>
       <c r="B249" s="2" t="s">
         <v>243</v>
       </c>
-    </row>
-    <row r="250" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J249" s="2"/>
+      <c r="K249" s="2"/>
+    </row>
+    <row r="250" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A250" s="2">
         <v>236</v>
       </c>
@@ -4940,35 +5478,43 @@
       <c r="G250" s="2" t="s">
         <v>474</v>
       </c>
-      <c r="I250" s="2" t="s">
+      <c r="J250" s="2"/>
+      <c r="K250" s="2"/>
+      <c r="L250" s="2" t="s">
         <v>475</v>
       </c>
     </row>
-    <row r="251" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A251" s="2">
         <v>237</v>
       </c>
       <c r="B251" s="2" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="252" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J251" s="2"/>
+      <c r="K251" s="2"/>
+    </row>
+    <row r="252" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A252" s="2">
         <v>238</v>
       </c>
       <c r="B252" s="2" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="253" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J252" s="2"/>
+      <c r="K252" s="2"/>
+    </row>
+    <row r="253" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A253" s="2">
         <v>239</v>
       </c>
       <c r="B253" s="2" t="s">
         <v>247</v>
       </c>
-    </row>
-    <row r="254" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J253" s="2"/>
+      <c r="K253" s="2"/>
+    </row>
+    <row r="254" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A254" s="2">
         <v>240</v>
       </c>
@@ -4990,515 +5536,643 @@
       <c r="G254" s="2" t="s">
         <v>369</v>
       </c>
-      <c r="I254" s="2" t="s">
+      <c r="J254" s="2"/>
+      <c r="K254" s="2"/>
+      <c r="L254" s="2" t="s">
         <v>479</v>
       </c>
     </row>
-    <row r="255" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A255" s="2">
         <v>241</v>
       </c>
       <c r="B255" s="2" t="s">
         <v>250</v>
       </c>
-    </row>
-    <row r="256" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J255" s="2"/>
+      <c r="K255" s="2"/>
+    </row>
+    <row r="256" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A256" s="2">
         <v>242</v>
       </c>
       <c r="B256" s="2" t="s">
         <v>249</v>
       </c>
-    </row>
-    <row r="257" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J256" s="2"/>
+      <c r="K256" s="2"/>
+    </row>
+    <row r="257" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A257" s="2">
         <v>243</v>
       </c>
       <c r="B257" s="2" t="s">
         <v>251</v>
       </c>
-    </row>
-    <row r="258" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J257" s="2"/>
+      <c r="K257" s="2"/>
+    </row>
+    <row r="258" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A258" s="2">
         <v>244</v>
       </c>
       <c r="B258" s="2" t="s">
         <v>252</v>
       </c>
-    </row>
-    <row r="259" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J258" s="2"/>
+      <c r="K258" s="2"/>
+    </row>
+    <row r="259" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A259" s="2">
         <v>245</v>
       </c>
       <c r="B259" s="2" t="s">
         <v>256</v>
       </c>
-    </row>
-    <row r="260" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J259" s="2"/>
+      <c r="K259" s="2"/>
+    </row>
+    <row r="260" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A260" s="2">
         <v>246</v>
       </c>
       <c r="B260" s="2" t="s">
         <v>254</v>
       </c>
-    </row>
-    <row r="261" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J260" s="2"/>
+      <c r="K260" s="2"/>
+    </row>
+    <row r="261" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A261" s="2">
         <v>247</v>
       </c>
       <c r="B261" s="2" t="s">
         <v>255</v>
       </c>
-    </row>
-    <row r="262" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J261" s="2"/>
+      <c r="K261" s="2"/>
+    </row>
+    <row r="262" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A262" s="2">
         <v>248</v>
       </c>
       <c r="B262" s="2" t="s">
         <v>253</v>
       </c>
-    </row>
-    <row r="263" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J262" s="2"/>
+      <c r="K262" s="2"/>
+    </row>
+    <row r="263" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A263" s="2">
         <v>249</v>
       </c>
       <c r="B263" s="2" t="s">
         <v>258</v>
       </c>
-    </row>
-    <row r="264" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J263" s="2"/>
+      <c r="K263" s="2"/>
+    </row>
+    <row r="264" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A264" s="2">
         <v>250</v>
       </c>
       <c r="B264" s="2" t="s">
         <v>259</v>
       </c>
-    </row>
-    <row r="265" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J264" s="2"/>
+      <c r="K264" s="2"/>
+    </row>
+    <row r="265" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A265" s="2">
         <v>251</v>
       </c>
       <c r="B265" s="2" t="s">
         <v>263</v>
       </c>
-    </row>
-    <row r="266" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J265" s="2"/>
+      <c r="K265" s="2"/>
+    </row>
+    <row r="266" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A266" s="2">
         <v>252</v>
       </c>
       <c r="B266" s="2" t="s">
         <v>257</v>
       </c>
-    </row>
-    <row r="267" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J266" s="2"/>
+      <c r="K266" s="2"/>
+    </row>
+    <row r="267" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A267" s="2">
         <v>253</v>
       </c>
       <c r="B267" s="2" t="s">
         <v>260</v>
       </c>
-    </row>
-    <row r="268" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J267" s="2"/>
+      <c r="K267" s="2"/>
+    </row>
+    <row r="268" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A268" s="2">
         <v>254</v>
       </c>
       <c r="B268" s="2" t="s">
         <v>261</v>
       </c>
-    </row>
-    <row r="269" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J268" s="2"/>
+      <c r="K268" s="2"/>
+    </row>
+    <row r="269" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A269" s="2">
         <v>255</v>
       </c>
       <c r="B269" s="2" t="s">
         <v>262</v>
       </c>
-    </row>
-    <row r="270" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J269" s="2"/>
+      <c r="K269" s="2"/>
+    </row>
+    <row r="270" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A270" s="2">
         <v>256</v>
       </c>
       <c r="B270" s="2" t="s">
         <v>264</v>
       </c>
-    </row>
-    <row r="271" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J270" s="2"/>
+      <c r="K270" s="2"/>
+    </row>
+    <row r="271" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A271" s="2">
         <v>257</v>
       </c>
       <c r="B271" s="2" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="272" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J271" s="2"/>
+      <c r="K271" s="2"/>
+    </row>
+    <row r="272" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A272" s="2">
         <v>258</v>
       </c>
       <c r="B272" s="2" t="s">
         <v>266</v>
       </c>
-    </row>
-    <row r="273" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J272" s="2"/>
+      <c r="K272" s="2"/>
+    </row>
+    <row r="273" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A273" s="2">
         <v>259</v>
       </c>
       <c r="B273" s="2" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="274" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J273" s="2"/>
+      <c r="K273" s="2"/>
+    </row>
+    <row r="274" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A274" s="2">
         <v>260</v>
       </c>
       <c r="B274" s="2" t="s">
         <v>268</v>
       </c>
-    </row>
-    <row r="275" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J274" s="2"/>
+      <c r="K274" s="2"/>
+    </row>
+    <row r="275" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A275" s="2">
         <v>261</v>
       </c>
       <c r="B275" s="2" t="s">
         <v>269</v>
       </c>
-    </row>
-    <row r="276" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J275" s="2"/>
+      <c r="K275" s="2"/>
+    </row>
+    <row r="276" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A276" s="2">
         <v>262</v>
       </c>
       <c r="B276" s="2" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="277" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J276" s="2"/>
+      <c r="K276" s="2"/>
+    </row>
+    <row r="277" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A277" s="2">
         <v>263</v>
       </c>
       <c r="B277" s="2" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="278" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J277" s="2"/>
+      <c r="K277" s="2"/>
+    </row>
+    <row r="278" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A278" s="2">
         <v>264</v>
       </c>
       <c r="B278" s="2" t="s">
         <v>272</v>
       </c>
-    </row>
-    <row r="279" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J278" s="2"/>
+      <c r="K278" s="2"/>
+    </row>
+    <row r="279" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A279" s="2">
         <v>265</v>
       </c>
       <c r="B279" s="2" t="s">
         <v>273</v>
       </c>
-    </row>
-    <row r="280" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J279" s="2"/>
+      <c r="K279" s="2"/>
+    </row>
+    <row r="280" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A280" s="2">
         <v>266</v>
       </c>
       <c r="B280" s="2" t="s">
         <v>274</v>
       </c>
-    </row>
-    <row r="281" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J280" s="2"/>
+      <c r="K280" s="2"/>
+    </row>
+    <row r="281" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A281" s="2">
         <v>267</v>
       </c>
       <c r="B281" s="2" t="s">
         <v>275</v>
       </c>
-    </row>
-    <row r="282" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J281" s="2"/>
+      <c r="K281" s="2"/>
+    </row>
+    <row r="282" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A282" s="2">
         <v>268</v>
       </c>
       <c r="B282" s="2" t="s">
         <v>276</v>
       </c>
-    </row>
-    <row r="283" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J282" s="2"/>
+      <c r="K282" s="2"/>
+    </row>
+    <row r="283" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A283" s="2">
         <v>269</v>
       </c>
       <c r="B283" s="2" t="s">
         <v>277</v>
       </c>
-    </row>
-    <row r="284" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J283" s="2"/>
+      <c r="K283" s="2"/>
+    </row>
+    <row r="284" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A284" s="2">
         <v>270</v>
       </c>
       <c r="B284" s="2" t="s">
         <v>278</v>
       </c>
-    </row>
-    <row r="285" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J284" s="2"/>
+      <c r="K284" s="2"/>
+    </row>
+    <row r="285" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A285" s="2">
         <v>271</v>
       </c>
       <c r="B285" s="2" t="s">
         <v>280</v>
       </c>
-    </row>
-    <row r="286" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J285" s="2"/>
+      <c r="K285" s="2"/>
+    </row>
+    <row r="286" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A286" s="2">
         <v>272</v>
       </c>
       <c r="B286" s="2" t="s">
         <v>281</v>
       </c>
-    </row>
-    <row r="287" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J286" s="2"/>
+      <c r="K286" s="2"/>
+    </row>
+    <row r="287" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A287" s="2">
         <v>273</v>
       </c>
       <c r="B287" s="2" t="s">
         <v>282</v>
       </c>
-    </row>
-    <row r="288" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J287" s="2"/>
+      <c r="K287" s="2"/>
+    </row>
+    <row r="288" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A288" s="2">
         <v>274</v>
       </c>
       <c r="B288" s="2" t="s">
         <v>283</v>
       </c>
-    </row>
-    <row r="289" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J288" s="2"/>
+      <c r="K288" s="2"/>
+    </row>
+    <row r="289" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A289" s="2">
         <v>275</v>
       </c>
       <c r="B289" s="2" t="s">
         <v>284</v>
       </c>
-    </row>
-    <row r="290" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J289" s="2"/>
+      <c r="K289" s="2"/>
+    </row>
+    <row r="290" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A290" s="2">
         <v>276</v>
       </c>
       <c r="B290" s="2" t="s">
         <v>285</v>
       </c>
-    </row>
-    <row r="291" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J290" s="2"/>
+      <c r="K290" s="2"/>
+    </row>
+    <row r="291" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A291" s="2">
         <v>277</v>
       </c>
       <c r="B291" s="2" t="s">
         <v>286</v>
       </c>
-    </row>
-    <row r="292" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J291" s="2"/>
+      <c r="K291" s="2"/>
+    </row>
+    <row r="292" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A292" s="2">
         <v>278</v>
       </c>
       <c r="B292" s="2" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="293" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J292" s="2"/>
+      <c r="K292" s="2"/>
+    </row>
+    <row r="293" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A293" s="2">
         <v>279</v>
       </c>
       <c r="B293" s="2" t="s">
         <v>287</v>
       </c>
-    </row>
-    <row r="294" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J293" s="2"/>
+      <c r="K293" s="2"/>
+    </row>
+    <row r="294" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A294" s="2">
         <v>280</v>
       </c>
       <c r="B294" s="2" t="s">
         <v>288</v>
       </c>
-    </row>
-    <row r="295" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J294" s="2"/>
+      <c r="K294" s="2"/>
+    </row>
+    <row r="295" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A295" s="2">
         <v>281</v>
       </c>
       <c r="B295" s="2" t="s">
         <v>289</v>
       </c>
-    </row>
-    <row r="296" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J295" s="2"/>
+      <c r="K295" s="2"/>
+    </row>
+    <row r="296" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A296" s="2">
         <v>282</v>
       </c>
       <c r="B296" s="2" t="s">
         <v>290</v>
       </c>
-    </row>
-    <row r="297" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J296" s="2"/>
+      <c r="K296" s="2"/>
+    </row>
+    <row r="297" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A297" s="2">
         <v>283</v>
       </c>
       <c r="B297" s="2" t="s">
         <v>291</v>
       </c>
-    </row>
-    <row r="298" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J297" s="2"/>
+      <c r="K297" s="2"/>
+    </row>
+    <row r="298" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A298" s="2">
         <v>284</v>
       </c>
       <c r="B298" s="2" t="s">
         <v>292</v>
       </c>
-    </row>
-    <row r="299" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J298" s="2"/>
+      <c r="K298" s="2"/>
+    </row>
+    <row r="299" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A299" s="2">
         <v>285</v>
       </c>
       <c r="B299" s="2" t="s">
         <v>293</v>
       </c>
-    </row>
-    <row r="300" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J299" s="2"/>
+      <c r="K299" s="2"/>
+    </row>
+    <row r="300" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A300" s="2">
         <v>286</v>
       </c>
       <c r="B300" s="2" t="s">
         <v>294</v>
       </c>
-    </row>
-    <row r="301" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J300" s="2"/>
+      <c r="K300" s="2"/>
+    </row>
+    <row r="301" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A301" s="2">
         <v>287</v>
       </c>
       <c r="B301" s="2" t="s">
         <v>296</v>
       </c>
-    </row>
-    <row r="302" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J301" s="2"/>
+      <c r="K301" s="2"/>
+    </row>
+    <row r="302" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A302" s="2">
         <v>288</v>
       </c>
       <c r="B302" s="2" t="s">
         <v>295</v>
       </c>
-    </row>
-    <row r="303" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J302" s="2"/>
+      <c r="K302" s="2"/>
+    </row>
+    <row r="303" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A303" s="2">
         <v>289</v>
       </c>
       <c r="B303" s="2" t="s">
         <v>297</v>
       </c>
-    </row>
-    <row r="304" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J303" s="2"/>
+      <c r="K303" s="2"/>
+    </row>
+    <row r="304" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A304" s="2">
         <v>290</v>
       </c>
       <c r="B304" s="2" t="s">
         <v>298</v>
       </c>
-    </row>
-    <row r="305" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J304" s="2"/>
+      <c r="K304" s="2"/>
+    </row>
+    <row r="305" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A305" s="2">
         <v>291</v>
       </c>
       <c r="B305" s="2" t="s">
         <v>299</v>
       </c>
-    </row>
-    <row r="306" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J305" s="2"/>
+      <c r="K305" s="2"/>
+    </row>
+    <row r="306" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A306" s="2">
         <v>292</v>
       </c>
       <c r="B306" s="2" t="s">
         <v>300</v>
       </c>
-    </row>
-    <row r="307" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J306" s="2"/>
+      <c r="K306" s="2"/>
+    </row>
+    <row r="307" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A307" s="2">
         <v>293</v>
       </c>
       <c r="B307" s="2" t="s">
         <v>301</v>
       </c>
-    </row>
-    <row r="308" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J307" s="2"/>
+      <c r="K307" s="2"/>
+    </row>
+    <row r="308" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A308" s="2">
         <v>294</v>
       </c>
       <c r="B308" s="2" t="s">
         <v>302</v>
       </c>
-    </row>
-    <row r="309" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J308" s="2"/>
+      <c r="K308" s="2"/>
+    </row>
+    <row r="309" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A309" s="2">
         <v>295</v>
       </c>
       <c r="B309" s="2" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="310" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J309" s="2"/>
+      <c r="K309" s="2"/>
+    </row>
+    <row r="310" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A310" s="2">
         <v>296</v>
       </c>
       <c r="B310" s="2" t="s">
         <v>304</v>
       </c>
-    </row>
-    <row r="311" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J310" s="2"/>
+      <c r="K310" s="2"/>
+    </row>
+    <row r="311" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A311" s="2">
         <v>297</v>
       </c>
       <c r="B311" s="2" t="s">
         <v>305</v>
       </c>
-    </row>
-    <row r="312" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J311" s="2"/>
+      <c r="K311" s="2"/>
+    </row>
+    <row r="312" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A312" s="2">
         <v>298</v>
       </c>
       <c r="B312" s="2" t="s">
         <v>306</v>
       </c>
-    </row>
-    <row r="313" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J312" s="2"/>
+      <c r="K312" s="2"/>
+    </row>
+    <row r="313" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A313" s="2">
         <v>299</v>
       </c>
       <c r="B313" s="2" t="s">
         <v>307</v>
       </c>
-    </row>
-    <row r="314" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J313" s="2"/>
+      <c r="K313" s="2"/>
+    </row>
+    <row r="314" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A314" s="2">
         <v>300</v>
       </c>
       <c r="B314" s="2" t="s">
         <v>308</v>
       </c>
-    </row>
-    <row r="315" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J314" s="2"/>
+      <c r="K314" s="2"/>
+    </row>
+    <row r="315" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A315" s="2">
         <v>301</v>
       </c>
       <c r="B315" s="2" t="s">
         <v>309</v>
       </c>
-    </row>
-    <row r="316" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J315" s="2"/>
+      <c r="K315" s="2"/>
+    </row>
+    <row r="316" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A316" s="2">
         <v>302</v>
       </c>
       <c r="B316" s="2" t="s">
         <v>310</v>
       </c>
-    </row>
-    <row r="317" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J316" s="2"/>
+      <c r="K316" s="2"/>
+    </row>
+    <row r="317" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A317" s="2">
         <v>303</v>
       </c>
       <c r="B317" s="2" t="s">
         <v>311</v>
       </c>
-    </row>
-    <row r="318" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J317" s="2"/>
+      <c r="K317" s="2"/>
+    </row>
+    <row r="318" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A318" s="2">
         <v>304</v>
       </c>
@@ -5520,83 +6194,103 @@
       <c r="G318" s="2" t="s">
         <v>363</v>
       </c>
-      <c r="I318" s="2" t="s">
+      <c r="J318" s="2"/>
+      <c r="K318" s="2"/>
+      <c r="L318" s="2" t="s">
         <v>485</v>
       </c>
     </row>
-    <row r="319" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A319" s="2">
         <v>305</v>
       </c>
       <c r="B319" s="2" t="s">
         <v>313</v>
       </c>
-    </row>
-    <row r="320" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J319" s="2"/>
+      <c r="K319" s="2"/>
+    </row>
+    <row r="320" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A320" s="2">
         <v>306</v>
       </c>
       <c r="B320" s="2" t="s">
         <v>314</v>
       </c>
-    </row>
-    <row r="321" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J320" s="2"/>
+      <c r="K320" s="2"/>
+    </row>
+    <row r="321" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A321" s="2">
         <v>307</v>
       </c>
       <c r="B321" s="2" t="s">
         <v>315</v>
       </c>
-    </row>
-    <row r="322" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J321" s="2"/>
+      <c r="K321" s="2"/>
+    </row>
+    <row r="322" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A322" s="2">
         <v>308</v>
       </c>
       <c r="B322" s="2" t="s">
         <v>316</v>
       </c>
-    </row>
-    <row r="323" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J322" s="2"/>
+      <c r="K322" s="2"/>
+    </row>
+    <row r="323" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A323" s="2">
         <v>309</v>
       </c>
       <c r="B323" s="2" t="s">
         <v>317</v>
       </c>
-    </row>
-    <row r="324" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J323" s="2"/>
+      <c r="K323" s="2"/>
+    </row>
+    <row r="324" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A324" s="2">
         <v>310</v>
       </c>
       <c r="B324" s="2" t="s">
         <v>318</v>
       </c>
-    </row>
-    <row r="325" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J324" s="2"/>
+      <c r="K324" s="2"/>
+    </row>
+    <row r="325" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A325" s="2">
         <v>311</v>
       </c>
       <c r="B325" s="2" t="s">
         <v>319</v>
       </c>
-    </row>
-    <row r="326" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J325" s="2"/>
+      <c r="K325" s="2"/>
+    </row>
+    <row r="326" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A326" s="2">
         <v>312</v>
       </c>
       <c r="B326" s="2" t="s">
         <v>320</v>
       </c>
-    </row>
-    <row r="327" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J326" s="2"/>
+      <c r="K326" s="2"/>
+    </row>
+    <row r="327" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A327" s="2">
         <v>313</v>
       </c>
       <c r="B327" s="2" t="s">
         <v>321</v>
       </c>
-    </row>
-    <row r="328" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J327" s="2"/>
+      <c r="K327" s="2"/>
+    </row>
+    <row r="328" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A328" s="2">
         <v>314</v>
       </c>
@@ -5618,11 +6312,13 @@
       <c r="H328" s="2" t="s">
         <v>493</v>
       </c>
-      <c r="I328" s="2" t="s">
+      <c r="J328" s="2"/>
+      <c r="K328" s="2"/>
+      <c r="L328" s="2" t="s">
         <v>485</v>
       </c>
     </row>
-    <row r="329" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A329" s="2">
         <v>315</v>
       </c>
@@ -5647,11 +6343,13 @@
       <c r="H329" s="2" t="s">
         <v>484</v>
       </c>
-      <c r="I329" s="2" t="s">
+      <c r="J329" s="2"/>
+      <c r="K329" s="2"/>
+      <c r="L329" s="2" t="s">
         <v>485</v>
       </c>
     </row>
-    <row r="330" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A330" s="2">
         <v>315</v>
       </c>
@@ -5673,35 +6371,43 @@
       <c r="H330" s="2" t="s">
         <v>488</v>
       </c>
-      <c r="I330" s="2" t="s">
+      <c r="J330" s="2"/>
+      <c r="K330" s="2"/>
+      <c r="L330" s="2" t="s">
         <v>485</v>
       </c>
     </row>
-    <row r="331" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A331" s="2">
         <v>316</v>
       </c>
       <c r="B331" s="2" t="s">
         <v>324</v>
       </c>
-    </row>
-    <row r="332" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J331" s="2"/>
+      <c r="K331" s="2"/>
+    </row>
+    <row r="332" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A332" s="2">
         <v>317</v>
       </c>
       <c r="B332" s="2" t="s">
         <v>325</v>
       </c>
-    </row>
-    <row r="333" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J332" s="2"/>
+      <c r="K332" s="2"/>
+    </row>
+    <row r="333" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A333" s="2">
         <v>318</v>
       </c>
       <c r="B333" s="2" t="s">
         <v>326</v>
       </c>
-    </row>
-    <row r="334" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J333" s="2"/>
+      <c r="K333" s="2"/>
+    </row>
+    <row r="334" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A334" s="2">
         <v>319</v>
       </c>
@@ -5723,123 +6429,153 @@
       <c r="H334" s="2" t="s">
         <v>531</v>
       </c>
-      <c r="I334" s="2" t="s">
+      <c r="J334" s="2"/>
+      <c r="K334" s="2"/>
+      <c r="L334" s="2" t="s">
         <v>485</v>
       </c>
     </row>
-    <row r="335" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A335" s="2">
         <v>320</v>
       </c>
       <c r="B335" s="2" t="s">
         <v>328</v>
       </c>
-    </row>
-    <row r="336" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J335" s="2"/>
+      <c r="K335" s="2"/>
+    </row>
+    <row r="336" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A336" s="2">
         <v>321</v>
       </c>
       <c r="B336" s="2" t="s">
         <v>329</v>
       </c>
-    </row>
-    <row r="337" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J336" s="2"/>
+      <c r="K336" s="2"/>
+    </row>
+    <row r="337" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A337" s="2">
         <v>322</v>
       </c>
       <c r="B337" s="2" t="s">
         <v>331</v>
       </c>
-    </row>
-    <row r="338" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J337" s="2"/>
+      <c r="K337" s="2"/>
+    </row>
+    <row r="338" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A338" s="2">
         <v>323</v>
       </c>
       <c r="B338" s="2" t="s">
         <v>330</v>
       </c>
-    </row>
-    <row r="339" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J338" s="2"/>
+      <c r="K338" s="2"/>
+    </row>
+    <row r="339" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A339" s="2">
         <v>324</v>
       </c>
       <c r="B339" s="2" t="s">
         <v>332</v>
       </c>
-    </row>
-    <row r="340" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J339" s="2"/>
+      <c r="K339" s="2"/>
+    </row>
+    <row r="340" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A340" s="2">
         <v>325</v>
       </c>
       <c r="B340" s="2" t="s">
         <v>333</v>
       </c>
-    </row>
-    <row r="341" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J340" s="2"/>
+      <c r="K340" s="2"/>
+    </row>
+    <row r="341" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A341" s="2">
         <v>326</v>
       </c>
       <c r="B341" s="2" t="s">
         <v>335</v>
       </c>
-    </row>
-    <row r="342" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J341" s="2"/>
+      <c r="K341" s="2"/>
+    </row>
+    <row r="342" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A342" s="2">
         <v>327</v>
       </c>
       <c r="B342" s="2" t="s">
         <v>336</v>
       </c>
-    </row>
-    <row r="343" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J342" s="2"/>
+      <c r="K342" s="2"/>
+    </row>
+    <row r="343" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A343" s="2">
         <v>328</v>
       </c>
       <c r="B343" s="2" t="s">
         <v>334</v>
       </c>
-    </row>
-    <row r="344" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J343" s="2"/>
+      <c r="K343" s="2"/>
+    </row>
+    <row r="344" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A344" s="2">
         <v>329</v>
       </c>
       <c r="B344" s="2" t="s">
         <v>337</v>
       </c>
-    </row>
-    <row r="345" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J344" s="2"/>
+      <c r="K344" s="2"/>
+    </row>
+    <row r="345" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A345" s="2">
         <v>330</v>
       </c>
       <c r="B345" s="2" t="s">
         <v>338</v>
       </c>
-    </row>
-    <row r="346" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J345" s="2"/>
+      <c r="K345" s="2"/>
+    </row>
+    <row r="346" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A346" s="2">
         <v>331</v>
       </c>
       <c r="B346" s="2" t="s">
         <v>339</v>
       </c>
-    </row>
-    <row r="347" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J346" s="2"/>
+      <c r="K346" s="2"/>
+    </row>
+    <row r="347" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A347" s="2">
         <v>332</v>
       </c>
       <c r="B347" s="2" t="s">
         <v>340</v>
       </c>
-    </row>
-    <row r="348" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J347" s="2"/>
+      <c r="K347" s="2"/>
+    </row>
+    <row r="348" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A348" s="2">
         <v>333</v>
       </c>
       <c r="B348" s="2" t="s">
         <v>341</v>
       </c>
-    </row>
-    <row r="349" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="J348" s="2"/>
+      <c r="K348" s="2"/>
+    </row>
+    <row r="349" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A349" s="5">
         <v>334</v>
       </c>
@@ -5864,23 +6600,28 @@
       <c r="H349" s="5" t="s">
         <v>530</v>
       </c>
-      <c r="I349" s="5" t="s">
+      <c r="J349" s="5"/>
+      <c r="K349" s="5"/>
+      <c r="L349" s="5" t="s">
         <v>427</v>
       </c>
     </row>
-    <row r="350" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A350" s="2">
         <v>335</v>
       </c>
       <c r="B350" s="2" t="s">
         <v>343</v>
       </c>
+      <c r="J350" s="2"/>
+      <c r="K350" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
-  <tableParts count="1">
+  <tableParts count="2">
     <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>